<commit_message>
change error checking to LOG_ERROR
</commit_message>
<xml_diff>
--- a/questions/Assignment6-ClientCommandTableForA7.xlsx
+++ b/questions/Assignment6-ClientCommandTableForA7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jiabinlin/SimplicityStudio/v5_workspace/ecen5823-assignment6-JiabinLin12/questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C75B44E-F84B-5740-A25B-C75961EEECE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ECBD93-0980-1E43-A9E2-DEB86FBAA20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -214,12 +214,6 @@
     <t>We get this event when it’s ok to call the next GATT command. It’s a good idea to check for returned error codes. This would be a great event to use to sequence your new state machine.</t>
   </si>
   <si>
-    <t xml:space="preserve"> save HTM service to data structure for rreference </t>
-  </si>
-  <si>
-    <t xml:space="preserve">save to HTM characteristic structure for reference </t>
-  </si>
-  <si>
     <t>Discovering the HTM service on the responder device</t>
   </si>
   <si>
@@ -233,6 +227,12 @@
   </si>
   <si>
     <t>Update for LCD discharge</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> save HTM service handle to data structure for rreference </t>
+  </si>
+  <si>
+    <t xml:space="preserve">save to HTM characteristic handle to structure for reference </t>
   </si>
 </sst>
 </file>
@@ -1676,8 +1676,8 @@
   </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="81" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1777,7 +1777,7 @@
         <v>14</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1789,7 +1789,7 @@
         <v>15</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1801,7 +1801,7 @@
         <v>16</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="26.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1837,7 +1837,7 @@
         <v>36</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1893,7 +1893,7 @@
         <v>37</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1967,7 +1967,7 @@
       <c r="C24" s="16"/>
       <c r="D24" s="16"/>
       <c r="E24" s="16" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="F24" s="16"/>
     </row>
@@ -1989,7 +1989,7 @@
       <c r="C26" s="16"/>
       <c r="D26" s="16"/>
       <c r="E26" s="16" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F26" s="16"/>
     </row>

</xml_diff>